<commit_message>
Ultimo commit dia 26/05 Blessed
</commit_message>
<xml_diff>
--- a/bancodedados.xlsx
+++ b/bancodedados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,24 +456,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PEdro</t>
+          <t>H2JKV</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PEdro</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
+        <v>12621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 tentativa de arrumar o bannco de daods
</commit_message>
<xml_diff>
--- a/bancodedados.xlsx
+++ b/bancodedados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,33 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>12621</v>
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>H2JKV</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>122333243</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>H2JKV</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>678568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>